<commit_message>
Data driven test case completed final
</commit_message>
<xml_diff>
--- a/target/classes/testData/VehicleInsuranceCalculator_TestData.xlsx
+++ b/target/classes/testData/VehicleInsuranceCalculator_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Workspace\Java_Training.InsuranceCalculator1\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972B4775-9FFD-4C3A-B8C2-B9CB5664319E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C689B8-4E52-4707-8307-FAC94132FA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>TC No</t>
   </si>
@@ -183,15 +183,15 @@
     <t>Verify Insurance Premium for Audi Moped</t>
   </si>
   <si>
+    <t>04/09/2019</t>
+  </si>
+  <si>
+    <t>04/09/2001</t>
+  </si>
+  <si>
     <t>04/09/1989</t>
   </si>
   <si>
-    <t>04/09/2001</t>
-  </si>
-  <si>
-    <t>04/09/2019</t>
-  </si>
-  <si>
     <t>12/12/1989</t>
   </si>
   <si>
@@ -201,16 +201,16 @@
     <t>12/12/1956</t>
   </si>
   <si>
-    <t>15/06/2023</t>
+    <t>06/15/2023</t>
+  </si>
+  <si>
+    <t>3000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,13 +261,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -607,9 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -618,20 +618,20 @@
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -643,88 +643,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -747,8 +747,8 @@
       <c r="F2">
         <v>666</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>55</v>
+      <c r="G2" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -765,7 +765,7 @@
       <c r="L2" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="N2" t="s">
@@ -786,11 +786,11 @@
       <c r="S2" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="U2">
-        <v>3000000</v>
+      <c r="U2" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="V2" t="s">
         <v>34</v>
@@ -807,7 +807,7 @@
       <c r="Z2" s="1">
         <v>1376</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="2">
         <v>2621</v>
       </c>
       <c r="AB2" t="s">
@@ -833,7 +833,7 @@
       <c r="F3">
         <v>900</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H3">
@@ -851,7 +851,7 @@
       <c r="L3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>57</v>
       </c>
       <c r="N3" t="s">
@@ -872,11 +872,11 @@
       <c r="S3" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="U3">
-        <v>3000000</v>
+      <c r="U3" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="V3" t="s">
         <v>34</v>
@@ -893,7 +893,7 @@
       <c r="Z3" s="1">
         <v>1379</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AA3" s="2">
         <v>2626</v>
       </c>
       <c r="AB3" t="s">
@@ -919,8 +919,8 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>53</v>
+      <c r="G4" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -937,7 +937,7 @@
       <c r="L4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="N4" t="s">
@@ -958,11 +958,11 @@
       <c r="S4" t="s">
         <v>42</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="U4">
-        <v>3000000</v>
+      <c r="U4" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="V4" t="s">
         <v>34</v>
@@ -985,25 +985,6 @@
       <c r="AB4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L8" s="2"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>